<commit_message>
close #48 created gender mapping for all files
test the full parsing - number of columns
</commit_message>
<xml_diff>
--- a/server/tests/files_to_test/students_list_excel/example_excel_english_non_regular_column_names.xlsx
+++ b/server/tests/files_to_test/students_list_excel/example_excel_english_non_regular_column_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar_Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\server\tests\files_to_test\students_list_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76056F1F-D153-4EF3-A742-701A85D10CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCFC4C4-2902-4552-9F62-D95D51D2015C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Idan Aviv</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Phone number</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -461,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949A20AF-119A-42AC-AEC9-B52646CBA3DA}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +492,7 @@
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -505,8 +517,11 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>528702484</v>
       </c>
@@ -531,8 +546,11 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>524291930</v>
       </c>
@@ -557,8 +575,11 @@
       <c r="H3" t="s">
         <v>15</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>526148959</v>
       </c>
@@ -583,8 +604,11 @@
       <c r="H4" t="s">
         <v>16</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>523454564</v>
       </c>
@@ -609,8 +633,11 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>530342423</v>
       </c>
@@ -635,8 +662,11 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>530342413</v>
       </c>
@@ -661,8 +691,11 @@
       <c r="H7" t="s">
         <v>19</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>537642324</v>
       </c>
@@ -686,6 +719,9 @@
       </c>
       <c r="H8" t="s">
         <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>